<commit_message>
Script para creacion de tablas y usuarios ampliado
</commit_message>
<xml_diff>
--- a/BBDD/Tranformación.xlsx
+++ b/BBDD/Tranformación.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1daw3\Desktop\programacion\TrabajoFinalMulti\BBDD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1daw3\Desktop\TrabajoTaller\BBDD\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
   <si>
     <t>CLIENTE</t>
   </si>
@@ -87,9 +87,6 @@
   </si>
   <si>
     <t>PIEZAS</t>
-  </si>
-  <si>
-    <t>Id_Facturas</t>
   </si>
   <si>
     <t>Id_Pieza</t>
@@ -534,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,7 +549,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -589,7 +586,7 @@
         <v>4</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>5</v>
@@ -628,16 +625,16 @@
         <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>7</v>
@@ -661,7 +658,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -671,10 +668,10 @@
         <v>20</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>8</v>
@@ -683,19 +680,19 @@
         <v>19</v>
       </c>
       <c r="F7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>2</v>
@@ -707,27 +704,27 @@
         <v>4</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -736,13 +733,13 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>

</xml_diff>